<commit_message>
Updated service entrance and calculations of installed and demand load for correct engine power
</commit_message>
<xml_diff>
--- a/Documentation/Sewage I & II/Carga Demandada.xlsx
+++ b/Documentation/Sewage I & II/Carga Demandada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AVTi\São Rafael I &amp; II\Documentation\Sewage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AVTi\São Rafael\Documentation\Sewage I &amp; II\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -606,7 +606,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A2" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -696,14 +696,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>17.45</v>
+        <v>18.41</v>
       </c>
       <c r="C6" s="16">
         <v>0.7</v>
       </c>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
-        <v>12.214999999999998</v>
+        <v>12.886999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24.95" customHeight="1" thickBot="1">
@@ -712,7 +712,7 @@
       </c>
       <c r="D7" s="15">
         <f>SUM(D2:D6)</f>
-        <v>19.39</v>
+        <v>20.061999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated calculations of installed and demand load for correct engine power
</commit_message>
<xml_diff>
--- a/Documentation/Sewage I & II/Carga Demandada.xlsx
+++ b/Documentation/Sewage I & II/Carga Demandada.xlsx
@@ -606,7 +606,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -696,14 +696,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>18.41</v>
+        <v>22.69</v>
       </c>
       <c r="C6" s="16">
         <v>0.7</v>
       </c>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
-        <v>12.886999999999999</v>
+        <v>15.882999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24.95" customHeight="1" thickBot="1">
@@ -712,7 +712,7 @@
       </c>
       <c r="D7" s="15">
         <f>SUM(D2:D6)</f>
-        <v>20.061999999999998</v>
+        <v>23.058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>